<commit_message>
checking kinds of input files
</commit_message>
<xml_diff>
--- a/Combo/features.xlsx
+++ b/Combo/features.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GLaPL/Combo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GSR_Learning/Combo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F81434-8B40-634B-BF50-47D738647291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E701E9D-D0DC-7F47-A357-076B7FFD4140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="460" windowWidth="27060" windowHeight="16040" activeTab="1" xr2:uid="{3BD78E3F-EBBF-E24C-8C1B-8FFA93325B4D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="98">
   <si>
     <t>﻿seg</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>aʊ</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>ʔ</t>
   </si>
 </sst>
 </file>
@@ -1031,14 +1037,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074B7588-5310-DB43-AEA5-121E2066FF91}">
-  <dimension ref="A1:AD42"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1760" ySplit="760" topLeftCell="C2" activePane="bottomRight"/>
+      <pane xSplit="1760" ySplit="760" topLeftCell="M16" activePane="bottomRight"/>
       <selection sqref="A1:A1048576"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
-      <selection pane="bottomRight" activeCell="AF42" sqref="AF42"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomRight" activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4271,6 +4277,71 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="X43">
+        <v>0</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>